<commit_message>
Se añaden headers a als celdas
</commit_message>
<xml_diff>
--- a/rickAndMorty.xlsx
+++ b/rickAndMorty.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,27 +422,29 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
-        <v>1</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Rick Sanchez</t>
+          <t>name</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Alive</t>
+          <t>status</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Morty Smith</t>
+          <t>Rick Sanchez</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -453,11 +455,11 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Summer Smith</t>
+          <t>Morty Smith</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -468,11 +470,11 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Beth Smith</t>
+          <t>Summer Smith</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -483,11 +485,11 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jerry Smith</t>
+          <t>Beth Smith</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -498,11 +500,11 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Abadango Cluster Princess</t>
+          <t>Jerry Smith</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -513,41 +515,41 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Abradolf Lincler</t>
+          <t>Abadango Cluster Princess</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Alive</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Adjudicator Rick</t>
+          <t>Abradolf Lincler</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Dead</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Agency Director</t>
+          <t>Adjudicator Rick</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -558,11 +560,11 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Alan Rails</t>
+          <t>Agency Director</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -573,11 +575,11 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Albert Einstein</t>
+          <t>Alan Rails</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -588,11 +590,11 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Alexander</t>
+          <t>Albert Einstein</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -603,26 +605,26 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Alien Googah</t>
+          <t>Alexander</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Dead</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Alien Morty</t>
+          <t>Alien Googah</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -633,11 +635,11 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Alien Rick</t>
+          <t>Alien Morty</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -648,41 +650,41 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Amish Cyborg</t>
+          <t>Alien Rick</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Dead</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Annie</t>
+          <t>Amish Cyborg</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Alive</t>
+          <t>Dead</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Antenna Morty</t>
+          <t>Annie</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -693,29 +695,44 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Antenna Rick</t>
+          <t>Antenna Morty</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Alive</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Antenna Rick</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
         <v>20</v>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>Ants in my Eyes Johnson</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>unknown</t>
         </is>

</xml_diff>